<commit_message>
get photo from local
</commit_message>
<xml_diff>
--- a/todo_report.xlsx
+++ b/todo_report.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,62 +424,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2020-02-04</t>
+          <t>2020-02-05</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15:41:35</t>
+          <t>09:53:55</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>507549293</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Kharisma Muzaki</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2020-02-05</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>09:53:55</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="n">
-        <v>14</v>
-      </c>
-      <c r="I3" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix passing data penugasan
</commit_message>
<xml_diff>
--- a/todo_report.xlsx
+++ b/todo_report.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,35 +379,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>tanggal tugas</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>terakhir submit</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tugas selesai</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>tugas belum selesai</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>diluar tugas</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>jumlah tugas</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>jumlah keseluruhan</t>
         </is>
@@ -424,27 +429,232 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>muzaki_gh</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>15:41:35</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>11</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>507549293</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kharisma Muzaki</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>muzaki_gh</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>2020-02-05</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>09:53:55</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F3" t="n">
         <v>4</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G3" t="n">
         <v>10</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I3" t="n">
         <v>14</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J3" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>123123087</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Harris Setyawan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>harris</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15:41:35</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J4" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3122331</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Riko Alfianto</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>riko</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>15:41:35</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>13</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>20</v>
+      </c>
+      <c r="J5" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>507123087</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Anada Badu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>anada</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>15:41:35</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>401123087</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mozaze</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>moza</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2020-02-04</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>15:41:35</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>13</v>
+      </c>
+      <c r="J7" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>